<commit_message>
Fix CSRF token issue in test question route
</commit_message>
<xml_diff>
--- a/questions1.xlsx
+++ b/questions1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF87A16-9CD1-4160-9A22-E3762A9EC336}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0727AF6-FB06-43CF-9EB4-57DDAD5F57CD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -659,8 +659,8 @@
   </sheetPr>
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AA22" sqref="AA22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -765,7 +765,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="150" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="131.25" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="93.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" ht="75" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="93.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="75" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>49</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="168.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="150" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>81</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="168.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="150" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>83</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="187.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="168.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>84</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>87</v>
       </c>
       <c r="O21" s="3">
-        <v>229.43</v>
+        <v>229.35</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>

</xml_diff>

<commit_message>
Renamed image files to remove spaces
</commit_message>
<xml_diff>
--- a/questions1.xlsx
+++ b/questions1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FE3929-4CC8-4058-9F18-C64A849DD74E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FA3A20-E036-4263-9147-BBA54956FEAB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -256,27 +256,12 @@
     <t>Який магнітний азимут встановлений на компасі?</t>
   </si>
   <si>
-    <t>Picture 1</t>
-  </si>
-  <si>
-    <t>Picture 5</t>
-  </si>
-  <si>
     <t>Визначте географічні координати вказаної точки. Широту та довготу вказувати градуси, хвилини та секунди через кому баз пробілів, наприклад, 52,37,40,31,37,20</t>
   </si>
   <si>
-    <t>Picture 2</t>
-  </si>
-  <si>
     <t>Визначте повні прямокутні координати вказаної точки. Координати осі абсцис Х та координати осі ординат Y вказувати через пробіл. Приклад: 5455500 5612750</t>
   </si>
   <si>
-    <t>Picture 3</t>
-  </si>
-  <si>
-    <t>Picture 4</t>
-  </si>
-  <si>
     <t>Чому буде дорівнювати азимут магнітний (Ам) якщо схилення на 2002 рік східне 10°15' (1-71), середнє відхилення меридіанів західне 2° 10' (0-36), а річна зміна схилення східна 0°04' (0-01)?</t>
   </si>
   <si>
@@ -286,9 +271,6 @@
     <t>Переведіть дирекційний кут направлення в азимут магнітний. Запишіть значення в градусах та хвилинах через кому. Приклад: 132,24</t>
   </si>
   <si>
-    <t>Picture 6</t>
-  </si>
-  <si>
     <t>Option 7</t>
   </si>
   <si>
@@ -347,6 +329,24 @@
   </si>
   <si>
     <t>singlechoice</t>
+  </si>
+  <si>
+    <t>Picture1</t>
+  </si>
+  <si>
+    <t>Picture2</t>
+  </si>
+  <si>
+    <t>Picture3</t>
+  </si>
+  <si>
+    <t>Picture4</t>
+  </si>
+  <si>
+    <t>Picture5</t>
+  </si>
+  <si>
+    <t>Picture6</t>
   </si>
 </sst>
 </file>
@@ -638,8 +638,8 @@
   </sheetPr>
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA19" sqref="AA19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -686,58 +686,58 @@
         <v>71</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="T1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>72</v>
@@ -746,7 +746,7 @@
         <v>73</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="131.25" x14ac:dyDescent="0.3">
@@ -780,7 +780,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
       <c r="AA2" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB2" s="2">
         <v>2</v>
@@ -814,7 +814,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB3" s="2">
         <v>2</v>
@@ -890,7 +890,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB5" s="2">
         <v>2</v>
@@ -927,7 +927,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB6" s="2">
         <v>2</v>
@@ -964,7 +964,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB7" s="2">
         <v>2</v>
@@ -1001,7 +1001,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB8" s="2">
         <v>2</v>
@@ -1103,7 +1103,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB10" s="2">
         <v>2</v>
@@ -1140,7 +1140,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB11" s="2">
         <v>2</v>
@@ -1177,7 +1177,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB12" s="2">
         <v>2</v>
@@ -1214,7 +1214,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB13" s="2">
         <v>2</v>
@@ -1251,7 +1251,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB14" s="2">
         <v>2</v>
@@ -1288,7 +1288,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB15" s="2">
         <v>2</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="16" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>77</v>
@@ -1324,10 +1324,10 @@
     </row>
     <row r="17" spans="1:28" ht="150" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>59</v>
@@ -1352,10 +1352,10 @@
     </row>
     <row r="18" spans="1:28" ht="150" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>60</v>
@@ -1380,10 +1380,10 @@
     </row>
     <row r="19" spans="1:28" ht="168.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>61</v>
@@ -1412,7 +1412,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB19" s="2">
         <v>3</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="20" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O20" s="3">
         <v>240</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="21" spans="1:28" ht="131.25" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="O21" s="3">
         <v>229.35</v>

</xml_diff>

<commit_message>
Fixed matching item heights on mobile devices
</commit_message>
<xml_diff>
--- a/questions1.xlsx
+++ b/questions1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CA1E07-A5D3-45FA-844A-DCEB760BCFA0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D993DDF1-B628-4882-B9E0-91B78C076C20}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -696,8 +696,8 @@
   </sheetPr>
   <dimension ref="A1:AC671"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update progress bar circle sizes based on screen width
</commit_message>
<xml_diff>
--- a/questions1.xlsx
+++ b/questions1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE7E125-D4B5-42F6-B14F-18D44BFDE9EB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F5C954-D585-4CFB-B296-3B6AECEA4412}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="406">
   <si>
     <t>Question</t>
   </si>
@@ -679,9 +679,6 @@
     <t>Охолодження ствола</t>
   </si>
   <si>
-    <t>З чого складаэться набой?</t>
-  </si>
-  <si>
     <t>Затвор</t>
   </si>
   <si>
@@ -994,9 +991,6 @@
     <t>Фіксацію магазину</t>
   </si>
   <si>
-    <t>Які дії виконує співробітник після команди «ПРИГОТУВАТИСЬ» з пістолетом?</t>
-  </si>
-  <si>
     <t>Вилучає пістолет з кобури</t>
   </si>
   <si>
@@ -1235,6 +1229,15 @@
   </si>
   <si>
     <t>Розібрати затворну групу</t>
+  </si>
+  <si>
+    <t>Cаундмодератори</t>
+  </si>
+  <si>
+    <t>З чого складається набой?</t>
+  </si>
+  <si>
+    <t>Які дії виконує співробітник після команди ПРИГОТУВАТИСЬ з пістолетом?</t>
   </si>
 </sst>
 </file>
@@ -1521,8 +1524,8 @@
   </sheetPr>
   <dimension ref="A1:AC720"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2238,25 +2241,25 @@
     </row>
     <row r="15" spans="1:29" s="4" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="E15" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>396</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>398</v>
       </c>
       <c r="AA15" s="4" t="s">
         <v>108</v>
@@ -2726,7 +2729,7 @@
         <v>212</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>214</v>
@@ -2744,7 +2747,7 @@
         <v>214</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="AA31" s="4" t="s">
         <v>9</v>
@@ -2793,37 +2796,37 @@
     </row>
     <row r="33" spans="2:28" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="H33" s="4" t="s">
-        <v>225</v>
-      </c>
       <c r="O33" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P33" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="P33" s="4" t="s">
-        <v>222</v>
-      </c>
       <c r="Q33" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="R33" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="R33" s="4" t="s">
-        <v>225</v>
       </c>
       <c r="AA33" s="4" t="s">
         <v>9</v>
@@ -2834,34 +2837,34 @@
     </row>
     <row r="34" spans="2:28" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>181</v>
       </c>
       <c r="D34" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>228</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>183</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>185</v>
       </c>
       <c r="O34" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="P34" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="P34" s="4" t="s">
+      <c r="Q34" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="Q34" s="4" t="s">
-        <v>229</v>
       </c>
       <c r="AA34" s="4" t="s">
         <v>9</v>
@@ -2872,34 +2875,34 @@
     </row>
     <row r="35" spans="2:28" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>231</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="G35" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="H35" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="H35" s="4" t="s">
-        <v>235</v>
-      </c>
       <c r="O35" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="P35" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="P35" s="4" t="s">
-        <v>232</v>
-      </c>
       <c r="Q35" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA35" s="4" t="s">
         <v>9</v>
@@ -2910,34 +2913,34 @@
     </row>
     <row r="36" spans="2:28" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="E36" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="F36" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>241</v>
-      </c>
       <c r="O36" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="P36" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="P36" s="4" t="s">
+      <c r="Q36" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="Q36" s="4" t="s">
-        <v>239</v>
-      </c>
       <c r="R36" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AA36" s="4" t="s">
         <v>9</v>
@@ -2948,7 +2951,7 @@
     </row>
     <row r="37" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>213</v>
@@ -2957,22 +2960,22 @@
         <v>210</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>211</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O37" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P37" s="4" t="s">
         <v>211</v>
       </c>
       <c r="Q37" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AA37" s="4" t="s">
         <v>9</v>
@@ -2983,31 +2986,31 @@
     </row>
     <row r="38" spans="2:28" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="G38" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q38" s="4" t="s">
         <v>238</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="O38" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="P38" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q38" s="4" t="s">
-        <v>239</v>
       </c>
       <c r="AA38" s="4" t="s">
         <v>9</v>
@@ -3018,10 +3021,10 @@
     </row>
     <row r="39" spans="2:28" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>215</v>
@@ -3030,25 +3033,25 @@
         <v>212</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>213</v>
       </c>
       <c r="O39" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="P39" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="P39" s="4" t="s">
+      <c r="Q39" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="Q39" s="4" t="s">
-        <v>252</v>
-      </c>
       <c r="R39" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S39" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AA39" s="4" t="s">
         <v>99</v>
@@ -3059,25 +3062,25 @@
     </row>
     <row r="40" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="G40" s="4" t="s">
-        <v>259</v>
-      </c>
       <c r="O40" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AA40" s="4" t="s">
         <v>108</v>
@@ -3088,25 +3091,25 @@
     </row>
     <row r="41" spans="2:28" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>264</v>
-      </c>
       <c r="O41" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA41" s="4" t="s">
         <v>108</v>
@@ -3117,25 +3120,25 @@
     </row>
     <row r="42" spans="2:28" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>272</v>
-      </c>
       <c r="O42" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AA42" s="4" t="s">
         <v>108</v>
@@ -3146,25 +3149,25 @@
     </row>
     <row r="43" spans="2:28" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="G43" s="4" t="s">
-        <v>278</v>
-      </c>
       <c r="O43" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA43" s="4" t="s">
         <v>108</v>
@@ -3175,25 +3178,25 @@
     </row>
     <row r="44" spans="2:28" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="G44" s="4" t="s">
-        <v>283</v>
-      </c>
       <c r="O44" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AA44" s="4" t="s">
         <v>108</v>
@@ -3204,25 +3207,25 @@
     </row>
     <row r="45" spans="2:28" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="F45" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="O45" s="4" t="s">
         <v>285</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="O45" s="4" t="s">
-        <v>286</v>
       </c>
       <c r="AA45" s="4" t="s">
         <v>108</v>
@@ -3233,25 +3236,25 @@
     </row>
     <row r="46" spans="2:28" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="G46" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>295</v>
-      </c>
       <c r="O46" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AA46" s="4" t="s">
         <v>108</v>
@@ -3262,25 +3265,25 @@
     </row>
     <row r="47" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="D47" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="F47" s="4" t="s">
+      <c r="G47" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>299</v>
-      </c>
       <c r="O47" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AA47" s="4" t="s">
         <v>108</v>
@@ -3291,25 +3294,25 @@
     </row>
     <row r="48" spans="2:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="E48" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="G48" s="4" t="s">
-        <v>305</v>
-      </c>
       <c r="O48" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AA48" s="4" t="s">
         <v>108</v>
@@ -3320,25 +3323,25 @@
     </row>
     <row r="49" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="G49" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="G49" s="4" t="s">
-        <v>312</v>
-      </c>
       <c r="O49" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA49" s="4" t="s">
         <v>108</v>
@@ -3349,25 +3352,25 @@
     </row>
     <row r="50" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="G50" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>318</v>
-      </c>
       <c r="O50" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AA50" s="4" t="s">
         <v>108</v>
@@ -3376,27 +3379,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>322</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>323</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>181</v>
       </c>
       <c r="O51" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AA51" s="4" t="s">
         <v>108</v>
@@ -3405,39 +3408,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" s="4" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="F52" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="G52" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="H52" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="G52" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>330</v>
-      </c>
       <c r="O52" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="P52" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q52" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="P52" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q52" s="4" t="s">
-        <v>327</v>
-      </c>
       <c r="R52" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AA52" s="4" t="s">
         <v>9</v>
@@ -3448,37 +3451,37 @@
     </row>
     <row r="53" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="E53" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="F53" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="G53" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="H53" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="F53" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>336</v>
-      </c>
       <c r="O53" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="P53" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q53" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="P53" s="4" t="s">
+      <c r="R53" s="4" t="s">
         <v>333</v>
-      </c>
-      <c r="Q53" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="R53" s="4" t="s">
-        <v>335</v>
       </c>
       <c r="AA53" s="4" t="s">
         <v>9</v>
@@ -3489,37 +3492,37 @@
     </row>
     <row r="54" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="G54" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="D54" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F54" s="4" t="s">
+      <c r="H54" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="G54" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>341</v>
-      </c>
       <c r="O54" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P54" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q54" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="R54" s="4" t="s">
         <v>339</v>
-      </c>
-      <c r="R54" s="4" t="s">
-        <v>341</v>
       </c>
       <c r="AA54" s="4" t="s">
         <v>9</v>
@@ -3530,37 +3533,37 @@
     </row>
     <row r="55" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="O55" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="P55" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="E55" s="4" t="s">
+      <c r="Q55" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="R55" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="S55" s="4" t="s">
         <v>346</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="O55" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="P55" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="Q55" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="R55" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="S55" s="4" t="s">
-        <v>348</v>
       </c>
       <c r="AA55" s="4" t="s">
         <v>99</v>
@@ -3571,37 +3574,37 @@
     </row>
     <row r="56" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="O56" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="P56" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="O56" s="4" t="s">
+      <c r="Q56" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="P56" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q56" s="4" t="s">
+      <c r="R56" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="R56" s="4" t="s">
+      <c r="S56" s="4" t="s">
         <v>354</v>
-      </c>
-      <c r="S56" s="4" t="s">
-        <v>356</v>
       </c>
       <c r="AA56" s="4" t="s">
         <v>99</v>
@@ -3612,37 +3615,37 @@
     </row>
     <row r="57" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="D57" s="4" t="s">
+      <c r="E57" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="F57" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="G57" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="G57" s="4" t="s">
-        <v>365</v>
-      </c>
       <c r="O57" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="P57" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="P57" s="4" t="s">
+      <c r="Q57" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="Q57" s="4" t="s">
+      <c r="R57" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="R57" s="4" t="s">
+      <c r="S57" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="S57" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="AA57" s="4" t="s">
         <v>99</v>
@@ -3653,37 +3656,37 @@
     </row>
     <row r="58" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="O58" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="O58" s="4" t="s">
+      <c r="P58" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="P58" s="4" t="s">
+      <c r="Q58" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="Q58" s="4" t="s">
+      <c r="R58" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="R58" s="4" t="s">
+      <c r="S58" s="4" t="s">
         <v>375</v>
-      </c>
-      <c r="S58" s="4" t="s">
-        <v>377</v>
       </c>
       <c r="AA58" s="4" t="s">
         <v>99</v>
@@ -3694,40 +3697,40 @@
     </row>
     <row r="59" spans="1:28" s="4" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C59" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="D59" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="E59" s="4" t="s">
+      <c r="G59" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="F59" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>281</v>
-      </c>
       <c r="O59" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P59" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="Q59" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R59" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="S59" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AA59" s="4" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="AB59" s="4">
         <v>3</v>
@@ -3735,43 +3738,43 @@
     </row>
     <row r="60" spans="1:28" s="4" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="D60" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D60" s="4" t="s">
-        <v>385</v>
-      </c>
       <c r="E60" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="G60" s="4" t="s">
         <v>382</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>384</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>182</v>
       </c>
       <c r="O60" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="P60" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="Q60" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R60" s="4" t="s">
         <v>182</v>
       </c>
       <c r="S60" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="T60" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AA60" s="4" t="s">
         <v>15</v>
@@ -3782,37 +3785,37 @@
     </row>
     <row r="61" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>389</v>
-      </c>
       <c r="E61" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G61" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="O61" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="P61" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q61" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="R61" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="S61" s="4" t="s">
         <v>388</v>
-      </c>
-      <c r="O61" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="P61" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="Q61" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="R61" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="S61" s="4" t="s">
-        <v>390</v>
       </c>
       <c r="AA61" s="4" t="s">
         <v>15</v>
@@ -3823,37 +3826,37 @@
     </row>
     <row r="62" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="O62" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P62" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="Q62" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="R62" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="S62" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="AA62" s="4" t="s">
         <v>15</v>
@@ -3865,22 +3868,22 @@
     <row r="63" spans="1:28" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
@@ -3896,13 +3899,13 @@
         <v>91</v>
       </c>
       <c r="Q63" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="R63" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="S63" s="4" t="s">
         <v>402</v>
-      </c>
-      <c r="R63" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="S63" s="4" t="s">
-        <v>404</v>
       </c>
       <c r="T63" s="4"/>
       <c r="U63" s="4"/>
@@ -4028,7 +4031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="206.25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" ht="187.5" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Add pdfmake files and update app.js with fixes for test availability, login issues, and screenshot prevention
</commit_message>
<xml_diff>
--- a/questions1.xlsx
+++ b/questions1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F5C954-D585-4CFB-B296-3B6AECEA4412}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537AADB1-0E89-4EE5-B846-FD7BCF3CBD54}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1524,8 +1524,8 @@
   </sheetPr>
   <dimension ref="A1:AC720"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="T55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3350,7 +3350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="4" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
         <v>312</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
         <v>365</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="4" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="4" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
         <v>384</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="s">
         <v>385</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
         <v>389</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>92</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>401</v>
+        <v>91</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>401</v>
@@ -4031,7 +4031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="187.5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" ht="206.25" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Show result page after test timer ends, fix saving error, enable PDF export
</commit_message>
<xml_diff>
--- a/questions1.xlsx
+++ b/questions1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537AADB1-0E89-4EE5-B846-FD7BCF3CBD54}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1687AD-C2AE-45FD-855F-084EDEA86967}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1524,14 +1524,14 @@
   </sheetPr>
   <dimension ref="A1:AC720"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="2"/>
-    <col min="2" max="2" width="30.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="30" style="2" customWidth="1"/>
     <col min="5" max="5" width="35" style="2" customWidth="1"/>
@@ -1637,7 +1637,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="3" customFormat="1" ht="152.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" s="3" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>81</v>
@@ -1696,7 +1696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>30</v>
@@ -1742,7 +1742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>35</v>
@@ -1788,7 +1788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="112.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>40</v>
@@ -1834,7 +1834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="112.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>45</v>
@@ -2017,7 +2017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="196.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>59</v>
@@ -2066,7 +2066,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="187.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>109</v>
@@ -2115,7 +2115,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="187.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>110</v>
@@ -2164,7 +2164,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>64</v>
@@ -2210,7 +2210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:29" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>115</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:29" s="4" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>391</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>121</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:28" s="4" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:28" s="4" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>127</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:28" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>133</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:28" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>174</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:28" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>180</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:28" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
         <v>186</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:28" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>202</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:28" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>209</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:28" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:28" s="4" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>404</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:28" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>398</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:28" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>264</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="2:28" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:28" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
         <v>266</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="2:28" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:28" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>278</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:28" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:28" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>283</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="2:28" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:28" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>289</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="2:28" s="4" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:28" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>295</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="2:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:28" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>299</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" s="4" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>306</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="4" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
         <v>312</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
         <v>318</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="4" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>405</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
         <v>335</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="s">
         <v>340</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
         <v>347</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
         <v>355</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
         <v>365</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="4" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
         <v>384</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="4" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="4" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
         <v>379</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="s">
         <v>385</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" s="4" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
         <v>389</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4" t="s">
         <v>399</v>
@@ -3981,7 +3981,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4" t="s">
         <v>114</v>
@@ -4031,7 +4031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="206.25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" ht="201" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
         <v>96</v>

</xml_diff>